<commit_message>
not sure, been a minute
</commit_message>
<xml_diff>
--- a/raw-data/combined_raw.xlsx
+++ b/raw-data/combined_raw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ey239/Github/IMT/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50347773-11A3-4F48-9CA2-97B7CE33846B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14990896-2D68-3C4E-AF29-DE2F44DC2B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9500" yWindow="-25680" windowWidth="27660" windowHeight="16960" xr2:uid="{44130C46-F722-614A-9453-7AAB84BA8AED}"/>
   </bookViews>
@@ -1281,8 +1281,8 @@
   <dimension ref="A1:O361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q356" sqref="Q356"/>
+      <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M296" sqref="M296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13224,7 +13224,7 @@
       <c r="J254" s="7">
         <v>120.37</v>
       </c>
-      <c r="K254" s="7">
+      <c r="K254" s="10">
         <v>10.08</v>
       </c>
       <c r="L254">
@@ -13271,7 +13271,7 @@
       <c r="J255">
         <v>104.44</v>
       </c>
-      <c r="K255">
+      <c r="K255" s="10">
         <v>20.56</v>
       </c>
       <c r="L255" s="7">
@@ -13318,7 +13318,7 @@
       <c r="J256">
         <v>193.2</v>
       </c>
-      <c r="K256" s="7">
+      <c r="K256" s="10">
         <v>0</v>
       </c>
       <c r="L256">
@@ -13365,7 +13365,7 @@
       <c r="J257">
         <v>75.42</v>
       </c>
-      <c r="K257">
+      <c r="K257" s="10">
         <v>5.49</v>
       </c>
       <c r="L257">
@@ -13412,7 +13412,7 @@
       <c r="J258">
         <v>185.88</v>
       </c>
-      <c r="K258" s="7">
+      <c r="K258" s="10">
         <v>0.05</v>
       </c>
       <c r="L258">
@@ -13459,14 +13459,14 @@
       <c r="J259">
         <v>85.61</v>
       </c>
-      <c r="K259">
+      <c r="K259" s="10">
         <v>41.91</v>
       </c>
       <c r="L259">
         <v>38.229999999999997</v>
       </c>
       <c r="M259" s="7">
-        <v>80.139999999999986</v>
+        <v>80.14</v>
       </c>
       <c r="N259">
         <v>17</v>
@@ -13506,7 +13506,7 @@
       <c r="J260" s="7">
         <v>123.99</v>
       </c>
-      <c r="K260" s="7">
+      <c r="K260" s="10">
         <v>38.58</v>
       </c>
       <c r="L260">
@@ -13553,7 +13553,7 @@
       <c r="J261">
         <v>263.55</v>
       </c>
-      <c r="K261" s="7">
+      <c r="K261" s="10">
         <v>0</v>
       </c>
       <c r="L261" s="7">
@@ -13600,7 +13600,7 @@
       <c r="J262">
         <v>80.31</v>
       </c>
-      <c r="K262">
+      <c r="K262" s="10">
         <v>9.09</v>
       </c>
       <c r="L262">
@@ -13647,7 +13647,7 @@
       <c r="J263">
         <v>179</v>
       </c>
-      <c r="K263" s="7">
+      <c r="K263" s="10">
         <v>0</v>
       </c>
       <c r="L263">
@@ -13694,7 +13694,7 @@
       <c r="J264">
         <v>108.09</v>
       </c>
-      <c r="K264" s="7">
+      <c r="K264" s="10">
         <v>42.64</v>
       </c>
       <c r="L264">
@@ -13741,7 +13741,7 @@
       <c r="J265">
         <v>105.23</v>
       </c>
-      <c r="K265">
+      <c r="K265" s="10">
         <v>11.11</v>
       </c>
       <c r="L265">
@@ -13788,7 +13788,7 @@
       <c r="J266">
         <v>242.35</v>
       </c>
-      <c r="K266" s="7">
+      <c r="K266" s="10">
         <v>0</v>
       </c>
       <c r="L266" s="7">
@@ -13835,14 +13835,14 @@
       <c r="J267">
         <v>96.1</v>
       </c>
-      <c r="K267" s="16">
-        <v>106.53</v>
+      <c r="K267" s="15">
+        <v>21.22</v>
       </c>
       <c r="L267">
         <v>106.53</v>
       </c>
       <c r="M267" s="7">
-        <v>213.06</v>
+        <v>127.75</v>
       </c>
       <c r="N267">
         <v>21</v>
@@ -13882,7 +13882,7 @@
       <c r="J268">
         <v>122.56</v>
       </c>
-      <c r="K268">
+      <c r="K268" s="10">
         <v>20.92</v>
       </c>
       <c r="L268">
@@ -13929,14 +13929,14 @@
       <c r="J269">
         <v>103.03</v>
       </c>
-      <c r="K269">
+      <c r="K269" s="10">
         <v>31.09</v>
       </c>
       <c r="L269">
         <v>88.9</v>
       </c>
       <c r="M269" s="7">
-        <v>119.99000000000001</v>
+        <v>119.99</v>
       </c>
       <c r="N269">
         <v>28</v>
@@ -13976,7 +13976,7 @@
       <c r="J270">
         <v>130.06</v>
       </c>
-      <c r="K270" s="7">
+      <c r="K270" s="10">
         <v>0</v>
       </c>
       <c r="L270">
@@ -14023,7 +14023,7 @@
       <c r="J271">
         <v>103.73</v>
       </c>
-      <c r="K271">
+      <c r="K271" s="10">
         <v>56.24</v>
       </c>
       <c r="L271">
@@ -14070,7 +14070,7 @@
       <c r="J272">
         <v>186.51</v>
       </c>
-      <c r="K272" s="7">
+      <c r="K272" s="10">
         <v>0</v>
       </c>
       <c r="L272">
@@ -14117,7 +14117,7 @@
       <c r="J273" s="7">
         <v>295.02</v>
       </c>
-      <c r="K273" s="7">
+      <c r="K273" s="10">
         <v>0</v>
       </c>
       <c r="L273" s="7">
@@ -14164,14 +14164,14 @@
       <c r="J274" s="7">
         <v>122.54</v>
       </c>
-      <c r="K274">
+      <c r="K274" s="10">
         <v>18.670000000000002</v>
       </c>
       <c r="L274">
         <v>99.54</v>
       </c>
       <c r="M274" s="7">
-        <v>118.21000000000001</v>
+        <v>118.21</v>
       </c>
       <c r="N274">
         <v>20</v>
@@ -14211,7 +14211,7 @@
       <c r="J275">
         <v>130.38999999999999</v>
       </c>
-      <c r="K275" s="7">
+      <c r="K275" s="10">
         <v>0</v>
       </c>
       <c r="L275">
@@ -14258,7 +14258,7 @@
       <c r="J276">
         <v>134.19999999999999</v>
       </c>
-      <c r="K276" s="7">
+      <c r="K276" s="10">
         <v>3.76</v>
       </c>
       <c r="L276">
@@ -14305,7 +14305,7 @@
       <c r="J277">
         <v>160.47</v>
       </c>
-      <c r="K277">
+      <c r="K277" s="10">
         <v>13.44</v>
       </c>
       <c r="L277" s="7">
@@ -14352,7 +14352,7 @@
       <c r="J278">
         <v>89.71</v>
       </c>
-      <c r="K278">
+      <c r="K278" s="10">
         <v>34.67</v>
       </c>
       <c r="L278">
@@ -14399,7 +14399,7 @@
       <c r="J279">
         <v>219.83</v>
       </c>
-      <c r="K279" s="7">
+      <c r="K279" s="10">
         <v>0</v>
       </c>
       <c r="L279">
@@ -14446,7 +14446,7 @@
       <c r="J280">
         <v>71.56</v>
       </c>
-      <c r="K280">
+      <c r="K280" s="10">
         <v>36.39</v>
       </c>
       <c r="L280">
@@ -14493,7 +14493,7 @@
       <c r="J281">
         <v>154.22999999999999</v>
       </c>
-      <c r="K281">
+      <c r="K281" s="10">
         <v>16.09</v>
       </c>
       <c r="L281">
@@ -14540,7 +14540,7 @@
       <c r="J282">
         <v>197.69</v>
       </c>
-      <c r="K282">
+      <c r="K282" s="10">
         <v>26.45</v>
       </c>
       <c r="L282" s="7">
@@ -14587,7 +14587,7 @@
       <c r="J283">
         <v>152.5</v>
       </c>
-      <c r="K283" s="7">
+      <c r="K283" s="10">
         <v>0</v>
       </c>
       <c r="L283">
@@ -14634,7 +14634,7 @@
       <c r="J284">
         <v>160.32</v>
       </c>
-      <c r="K284">
+      <c r="K284" s="10">
         <v>4.8899999999999997</v>
       </c>
       <c r="L284">
@@ -14681,7 +14681,7 @@
       <c r="J285" s="7">
         <v>185.37</v>
       </c>
-      <c r="K285" s="7">
+      <c r="K285" s="10">
         <v>0</v>
       </c>
       <c r="L285">
@@ -14728,7 +14728,7 @@
       <c r="J286">
         <v>296.02</v>
       </c>
-      <c r="K286" s="7">
+      <c r="K286" s="10">
         <v>0</v>
       </c>
       <c r="L286" s="7">
@@ -14775,7 +14775,7 @@
       <c r="J287">
         <v>119.05</v>
       </c>
-      <c r="K287">
+      <c r="K287" s="10">
         <v>11.54</v>
       </c>
       <c r="L287">
@@ -14822,7 +14822,7 @@
       <c r="J288" s="7">
         <v>194.11</v>
       </c>
-      <c r="K288" s="7">
+      <c r="K288" s="10">
         <v>0</v>
       </c>
       <c r="L288">
@@ -14869,7 +14869,7 @@
       <c r="J289">
         <v>113.73</v>
       </c>
-      <c r="K289">
+      <c r="K289" s="10">
         <v>10.220000000000001</v>
       </c>
       <c r="L289">

</xml_diff>